<commit_message>
Doc: Updated tasks status and actual hours for tasks done
</commit_message>
<xml_diff>
--- a/Release Planning/Release3_ planning.xlsx
+++ b/Release Planning/Release3_ planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C7994E-33D5-4307-A863-6627AB823768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FEB873-D822-460A-8478-E4325BD00325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
   <si>
     <t>WP</t>
   </si>
@@ -347,7 +347,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +405,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -719,50 +731,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -781,15 +781,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -799,18 +790,43 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,8 +1048,8 @@
   </sheetPr>
   <dimension ref="A1:G1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C48" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1062,13 +1078,13 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="37"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="67" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1081,11 +1097,11 @@
         <v>4</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
+      <c r="A3" s="68"/>
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1096,11 +1112,11 @@
         <v>4</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1109,11 +1125,11 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1122,11 +1138,11 @@
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1135,11 +1151,11 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="48"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1148,11 +1164,11 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="37"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1161,11 +1177,11 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="37"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="48"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1176,11 +1192,11 @@
         <v>1</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1189,11 +1205,11 @@
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="37"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45"/>
+      <c r="A11" s="68"/>
       <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1204,11 +1220,11 @@
         <v>1</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="45"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1217,11 +1233,11 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1230,11 +1246,11 @@
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1243,11 +1259,11 @@
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1258,11 +1274,11 @@
         <v>1</v>
       </c>
       <c r="E15" s="8"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45"/>
+      <c r="A16" s="68"/>
       <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
@@ -1271,11 +1287,11 @@
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45"/>
+      <c r="A17" s="68"/>
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
@@ -1286,11 +1302,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
+      <c r="A18" s="68"/>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1300,12 +1316,14 @@
       <c r="D18" s="7">
         <v>0.5</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37"/>
+      <c r="E18" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="47"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="45"/>
+      <c r="A19" s="68"/>
       <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
@@ -1314,11 +1332,11 @@
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45"/>
+      <c r="A20" s="68"/>
       <c r="B20" s="5" t="s">
         <v>31</v>
       </c>
@@ -1328,12 +1346,14 @@
       <c r="D20" s="7">
         <v>0.5</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="37"/>
+      <c r="E20" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="46"/>
+      <c r="A21" s="69"/>
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
@@ -1342,8 +1362,8 @@
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
     </row>
     <row r="22" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
@@ -1351,11 +1371,11 @@
       <c r="C22" s="11"/>
       <c r="D22" s="12"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="57"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="51"/>
     </row>
     <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="70" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1368,13 +1388,13 @@
         <v>4</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="37"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="45"/>
+      <c r="A24" s="68"/>
       <c r="B24" s="5" t="s">
         <v>36</v>
       </c>
@@ -1385,13 +1405,13 @@
         <v>4</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="56" t="s">
+      <c r="F24" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="37"/>
+      <c r="G24" s="48"/>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="45"/>
+      <c r="A25" s="68"/>
       <c r="B25" s="5" t="s">
         <v>37</v>
       </c>
@@ -1400,11 +1420,11 @@
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="37"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="45"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="5" t="s">
         <v>38</v>
       </c>
@@ -1413,11 +1433,11 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="37"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="45"/>
+      <c r="A27" s="68"/>
       <c r="B27" s="5" t="s">
         <v>39</v>
       </c>
@@ -1426,11 +1446,11 @@
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="37"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="45"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="5" t="s">
         <v>40</v>
       </c>
@@ -1439,11 +1459,11 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="37"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="48"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="45"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="5" t="s">
         <v>41</v>
       </c>
@@ -1452,11 +1472,11 @@
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="45"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="5" t="s">
         <v>42</v>
       </c>
@@ -1466,12 +1486,16 @@
       <c r="D30" s="7">
         <v>3</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="37"/>
+      <c r="E30" s="8">
+        <v>3</v>
+      </c>
+      <c r="F30" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="81"/>
     </row>
     <row r="31" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="45"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="5" t="s">
         <v>43</v>
       </c>
@@ -1480,11 +1504,11 @@
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="37"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="48"/>
     </row>
     <row r="32" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="45"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="5" t="s">
         <v>44</v>
       </c>
@@ -1494,12 +1518,16 @@
       <c r="D32" s="7">
         <v>3</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="37"/>
+      <c r="E32" s="8">
+        <v>3</v>
+      </c>
+      <c r="F32" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="81"/>
     </row>
     <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="45"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="5" t="s">
         <v>45</v>
       </c>
@@ -1508,11 +1536,11 @@
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="37"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="48"/>
     </row>
     <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="5" t="s">
         <v>46</v>
       </c>
@@ -1521,11 +1549,11 @@
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="37"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="48"/>
     </row>
     <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="5" t="s">
         <v>47</v>
       </c>
@@ -1534,11 +1562,11 @@
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="37"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="48"/>
     </row>
     <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="5" t="s">
         <v>48</v>
       </c>
@@ -1549,11 +1577,11 @@
         <v>1</v>
       </c>
       <c r="E36" s="8"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="37"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="48"/>
     </row>
     <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="45"/>
+      <c r="A37" s="68"/>
       <c r="B37" s="5" t="s">
         <v>49</v>
       </c>
@@ -1562,11 +1590,11 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="37"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="48"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="45"/>
+      <c r="A38" s="68"/>
       <c r="B38" s="5" t="s">
         <v>50</v>
       </c>
@@ -1577,11 +1605,11 @@
         <v>1</v>
       </c>
       <c r="E38" s="8"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="37"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="48"/>
     </row>
     <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
+      <c r="A39" s="68"/>
       <c r="B39" s="5" t="s">
         <v>51</v>
       </c>
@@ -1592,11 +1620,11 @@
         <v>1</v>
       </c>
       <c r="E39" s="8"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="37"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="48"/>
     </row>
     <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
+      <c r="A40" s="68"/>
       <c r="B40" s="5" t="s">
         <v>52</v>
       </c>
@@ -1605,11 +1633,11 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="37"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="48"/>
     </row>
     <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="45"/>
+      <c r="A41" s="68"/>
       <c r="B41" s="5" t="s">
         <v>53</v>
       </c>
@@ -1620,11 +1648,11 @@
         <v>1</v>
       </c>
       <c r="E41" s="8"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="37"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="48"/>
     </row>
     <row r="42" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="46"/>
+      <c r="A42" s="69"/>
       <c r="B42" s="5" t="s">
         <v>54</v>
       </c>
@@ -1633,8 +1661,8 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="8"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="37"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="48"/>
     </row>
     <row r="43" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
@@ -1642,11 +1670,11 @@
       <c r="C43" s="16"/>
       <c r="D43" s="17"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="37"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="48"/>
     </row>
     <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="71" t="s">
         <v>55</v>
       </c>
       <c r="B44" s="19" t="s">
@@ -1656,12 +1684,12 @@
         <v>8</v>
       </c>
       <c r="D44" s="20"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="37"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="48"/>
     </row>
     <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="45"/>
+      <c r="A45" s="68"/>
       <c r="B45" s="19" t="s">
         <v>57</v>
       </c>
@@ -1669,12 +1697,12 @@
         <v>13</v>
       </c>
       <c r="D45" s="20"/>
-      <c r="E45" s="66"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="37"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="48"/>
     </row>
     <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="45"/>
+      <c r="A46" s="68"/>
       <c r="B46" s="19" t="s">
         <v>58</v>
       </c>
@@ -1682,12 +1710,12 @@
         <v>13</v>
       </c>
       <c r="D46" s="20"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="37"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="48"/>
     </row>
     <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="45"/>
+      <c r="A47" s="68"/>
       <c r="B47" s="19" t="s">
         <v>59</v>
       </c>
@@ -1697,31 +1725,31 @@
       <c r="D47" s="20">
         <v>1</v>
       </c>
-      <c r="E47" s="66">
+      <c r="E47" s="36">
         <v>1</v>
       </c>
-      <c r="F47" s="58" t="s">
+      <c r="F47" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="G47" s="59"/>
+      <c r="G47" s="78"/>
     </row>
     <row r="48" spans="1:7" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="45"/>
+      <c r="A48" s="68"/>
       <c r="B48" s="20"/>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="37"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="48"/>
     </row>
     <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="46"/>
+      <c r="A49" s="69"/>
       <c r="B49" s="20"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
-      <c r="E49" s="66"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="37"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="48"/>
     </row>
     <row r="50" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
@@ -1729,65 +1757,65 @@
       <c r="C50" s="16"/>
       <c r="D50" s="17"/>
       <c r="E50" s="18"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="37"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="68" t="s">
+      <c r="A51" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40" t="s">
+      <c r="B51" s="75"/>
+      <c r="C51" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="43">
+      <c r="D51" s="76">
         <v>3</v>
       </c>
-      <c r="E51" s="69"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="61"/>
+      <c r="E51" s="58"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="53"/>
     </row>
     <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="45"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="63"/>
+      <c r="A52" s="68"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="55"/>
     </row>
     <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="45"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="70"/>
-      <c r="F53" s="62"/>
-      <c r="G53" s="63"/>
+      <c r="A53" s="68"/>
+      <c r="B53" s="42"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="55"/>
     </row>
     <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="46"/>
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="71"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="65"/>
+      <c r="A54" s="69"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="57"/>
     </row>
     <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="48"/>
-      <c r="B55" s="49"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="37"/>
+      <c r="A55" s="73"/>
+      <c r="B55" s="74"/>
+      <c r="C55" s="74"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="74"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="48"/>
     </row>
     <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="50" t="s">
+      <c r="A56" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="51"/>
+      <c r="B56" s="40"/>
       <c r="C56" s="22" t="s">
         <v>62</v>
       </c>
@@ -1795,43 +1823,43 @@
         <v>63</v>
       </c>
       <c r="E56" s="23"/>
-      <c r="F56" s="54" t="s">
+      <c r="F56" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="G56" s="55"/>
+      <c r="G56" s="46"/>
     </row>
     <row r="57" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="52"/>
-      <c r="B57" s="41"/>
+      <c r="A57" s="41"/>
+      <c r="B57" s="42"/>
       <c r="C57" s="24" t="s">
         <v>35</v>
       </c>
       <c r="D57" s="25"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="74"/>
-      <c r="G57" s="75"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="61"/>
+      <c r="G57" s="62"/>
     </row>
     <row r="58" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="52"/>
-      <c r="B58" s="41"/>
+      <c r="A58" s="41"/>
+      <c r="B58" s="42"/>
       <c r="C58" s="26" t="s">
         <v>65</v>
       </c>
       <c r="D58" s="25"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="76"/>
-      <c r="G58" s="77"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="64"/>
     </row>
     <row r="59" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="53"/>
-      <c r="B59" s="42"/>
+      <c r="A59" s="43"/>
+      <c r="B59" s="44"/>
       <c r="C59" s="27" t="s">
         <v>66</v>
       </c>
       <c r="D59" s="25"/>
-      <c r="E59" s="73"/>
-      <c r="F59" s="78"/>
-      <c r="G59" s="79"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="66"/>
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F61" s="28"/>
@@ -5671,6 +5699,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D51:D54"/>
     <mergeCell ref="A56:B59"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="F17:G17"/>
@@ -5687,56 +5762,9 @@
     <mergeCell ref="A2:A21"/>
     <mergeCell ref="A23:A42"/>
     <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F21 F23:F42 F44:F49 F61:G1019 F51" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F23:F42 F44:F49 F61:G1019 F1:F21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Doing,Done,To do"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Doc: updated task status and Actual Hours for Release 4 planning task
</commit_message>
<xml_diff>
--- a/Release Planning/Release3_ planning.xlsx
+++ b/Release Planning/Release3_ planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D881CC-5B92-45A9-A28C-70208BE4B3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F40C44-889B-42F1-BE60-458B566AE54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WP" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
   <si>
     <t>WP</t>
   </si>
@@ -387,7 +387,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,12 +458,6 @@
       <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -714,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -780,76 +774,49 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -870,37 +837,55 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1123,8 +1108,8 @@
   </sheetPr>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1153,10 +1138,10 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
@@ -1165,7 +1150,7 @@
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="7">
@@ -1174,13 +1159,13 @@
       <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="32"/>
+      <c r="G2" s="46"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1193,13 +1178,13 @@
       <c r="E3" s="8">
         <v>1</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="32"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1212,13 +1197,13 @@
       <c r="E4" s="8">
         <v>1</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="32"/>
+      <c r="G4" s="46"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1231,13 +1216,13 @@
       <c r="E5" s="8">
         <v>0.75</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1250,13 +1235,13 @@
       <c r="E6" s="8">
         <v>1</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="46"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1269,13 +1254,13 @@
       <c r="E7" s="8">
         <v>0.75</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1288,13 +1273,13 @@
       <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="46"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1307,13 +1292,13 @@
       <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="46"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1326,13 +1311,13 @@
       <c r="E10" s="8">
         <v>2</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="46"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1345,13 +1330,13 @@
       <c r="E11" s="8">
         <v>1</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1364,13 +1349,13 @@
       <c r="E12" s="8">
         <v>0.5</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="46"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1383,13 +1368,13 @@
       <c r="E13" s="8">
         <v>0.5</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="46"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1402,13 +1387,13 @@
       <c r="E14" s="8">
         <v>0.5</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="32"/>
+      <c r="G14" s="46"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1421,13 +1406,13 @@
       <c r="E15" s="8">
         <v>1</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
@@ -1440,13 +1425,13 @@
       <c r="E16" s="8">
         <v>0.5</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="32"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
+      <c r="A17" s="57"/>
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
@@ -1459,13 +1444,13 @@
       <c r="E17" s="8">
         <v>3</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="32"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1478,13 +1463,13 @@
       <c r="E18" s="8">
         <v>0.5</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="46"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
@@ -1497,13 +1482,13 @@
       <c r="E19" s="8">
         <v>0.5</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="32"/>
+      <c r="G19" s="46"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="5" t="s">
         <v>31</v>
       </c>
@@ -1516,13 +1501,13 @@
       <c r="E20" s="8">
         <v>0.5</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="32"/>
+      <c r="G20" s="46"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
@@ -1535,10 +1520,10 @@
       <c r="E21" s="8">
         <v>0.5</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="32"/>
+      <c r="G21" s="46"/>
     </row>
     <row r="22" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
@@ -1546,11 +1531,11 @@
       <c r="C22" s="11"/>
       <c r="D22" s="12"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="34"/>
+      <c r="F22" s="48"/>
       <c r="G22" s="49"/>
     </row>
     <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1565,13 +1550,13 @@
       <c r="E23" s="8">
         <v>4</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="46"/>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
+      <c r="A24" s="57"/>
       <c r="B24" s="5" t="s">
         <v>35</v>
       </c>
@@ -1584,13 +1569,13 @@
       <c r="E24" s="8">
         <v>6</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G24" s="59"/>
+      <c r="G24" s="47"/>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
@@ -1600,14 +1585,16 @@
       <c r="D25" s="7">
         <v>2.5</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="68"/>
+      <c r="E25" s="8">
+        <v>3</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="46"/>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+      <c r="A26" s="57"/>
       <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1620,13 +1607,13 @@
       <c r="E26" s="8">
         <v>2</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="46"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
+      <c r="A27" s="57"/>
       <c r="B27" s="5" t="s">
         <v>38</v>
       </c>
@@ -1636,14 +1623,16 @@
       <c r="D27" s="7">
         <v>2.5</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="68"/>
+      <c r="E27" s="8">
+        <v>3</v>
+      </c>
+      <c r="F27" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="46"/>
     </row>
     <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="5" t="s">
         <v>39</v>
       </c>
@@ -1656,13 +1645,13 @@
       <c r="E28" s="8">
         <v>2</v>
       </c>
-      <c r="F28" s="31" t="s">
+      <c r="F28" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="32"/>
+      <c r="G28" s="46"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="36"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="5" t="s">
         <v>40</v>
       </c>
@@ -1675,13 +1664,13 @@
       <c r="E29" s="8">
         <v>3</v>
       </c>
-      <c r="F29" s="31" t="s">
+      <c r="F29" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="G29" s="46"/>
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="5" t="s">
         <v>41</v>
       </c>
@@ -1694,13 +1683,13 @@
       <c r="E30" s="8">
         <v>3</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G30" s="32"/>
+      <c r="G30" s="46"/>
     </row>
     <row r="31" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="36"/>
+      <c r="A31" s="57"/>
       <c r="B31" s="5" t="s">
         <v>42</v>
       </c>
@@ -1713,13 +1702,13 @@
       <c r="E31" s="8">
         <v>3</v>
       </c>
-      <c r="F31" s="31" t="s">
+      <c r="F31" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="32"/>
+      <c r="G31" s="46"/>
     </row>
     <row r="32" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
+      <c r="A32" s="57"/>
       <c r="B32" s="5" t="s">
         <v>43</v>
       </c>
@@ -1732,13 +1721,13 @@
       <c r="E32" s="8">
         <v>3</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="32"/>
+      <c r="G32" s="46"/>
     </row>
     <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="57"/>
       <c r="B33" s="5" t="s">
         <v>44</v>
       </c>
@@ -1751,13 +1740,13 @@
       <c r="E33" s="8">
         <v>0.5</v>
       </c>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="32"/>
+      <c r="G33" s="46"/>
     </row>
     <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
+      <c r="A34" s="57"/>
       <c r="B34" s="5" t="s">
         <v>45</v>
       </c>
@@ -1770,13 +1759,13 @@
       <c r="E34" s="8">
         <v>0.5</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G34" s="32"/>
+      <c r="G34" s="46"/>
     </row>
     <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
+      <c r="A35" s="57"/>
       <c r="B35" s="5" t="s">
         <v>46</v>
       </c>
@@ -1786,14 +1775,16 @@
       <c r="D35" s="7">
         <v>0.5</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="G35" s="60"/>
+      <c r="E35" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F35" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="46"/>
     </row>
     <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
+      <c r="A36" s="57"/>
       <c r="B36" s="5" t="s">
         <v>47</v>
       </c>
@@ -1806,13 +1797,13 @@
       <c r="E36" s="8">
         <v>1</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="32"/>
+      <c r="G36" s="46"/>
     </row>
     <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
+      <c r="A37" s="57"/>
       <c r="B37" s="5" t="s">
         <v>48</v>
       </c>
@@ -1822,14 +1813,16 @@
       <c r="D37" s="7">
         <v>0.5</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="G37" s="60"/>
+      <c r="E37" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="G37" s="46"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
+      <c r="A38" s="57"/>
       <c r="B38" s="5" t="s">
         <v>49</v>
       </c>
@@ -1842,13 +1835,13 @@
       <c r="E38" s="8">
         <v>1</v>
       </c>
-      <c r="F38" s="31" t="s">
+      <c r="F38" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G38" s="32"/>
+      <c r="G38" s="46"/>
     </row>
     <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
+      <c r="A39" s="57"/>
       <c r="B39" s="5" t="s">
         <v>50</v>
       </c>
@@ -1861,13 +1854,13 @@
       <c r="E39" s="8">
         <v>1</v>
       </c>
-      <c r="F39" s="31" t="s">
+      <c r="F39" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G39" s="32"/>
+      <c r="G39" s="46"/>
     </row>
     <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="36"/>
+      <c r="A40" s="57"/>
       <c r="B40" s="5" t="s">
         <v>51</v>
       </c>
@@ -1880,13 +1873,13 @@
       <c r="E40" s="8">
         <v>1</v>
       </c>
-      <c r="F40" s="31" t="s">
+      <c r="F40" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G40" s="32"/>
+      <c r="G40" s="46"/>
     </row>
     <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="36"/>
+      <c r="A41" s="57"/>
       <c r="B41" s="5" t="s">
         <v>52</v>
       </c>
@@ -1899,13 +1892,13 @@
       <c r="E41" s="8">
         <v>1</v>
       </c>
-      <c r="F41" s="31" t="s">
+      <c r="F41" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G41" s="32"/>
+      <c r="G41" s="46"/>
     </row>
     <row r="42" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="37"/>
+      <c r="A42" s="58"/>
       <c r="B42" s="5" t="s">
         <v>53</v>
       </c>
@@ -1918,10 +1911,10 @@
       <c r="E42" s="8">
         <v>1</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G42" s="32"/>
+      <c r="G42" s="46"/>
     </row>
     <row r="43" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
@@ -1929,11 +1922,11 @@
       <c r="C43" s="16"/>
       <c r="D43" s="17"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="30"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="70"/>
     </row>
     <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="58" t="s">
+      <c r="A44" s="60" t="s">
         <v>54</v>
       </c>
       <c r="B44" s="19" t="s">
@@ -1948,13 +1941,13 @@
       <c r="E44" s="28">
         <v>2</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G44" s="32"/>
+      <c r="G44" s="46"/>
     </row>
     <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="36"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="19" t="s">
         <v>56</v>
       </c>
@@ -1967,13 +1960,13 @@
       <c r="E45" s="28">
         <v>1.1499999999999999</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G45" s="32"/>
+      <c r="G45" s="46"/>
     </row>
     <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="36"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="19" t="s">
         <v>57</v>
       </c>
@@ -1986,13 +1979,13 @@
       <c r="E46" s="28">
         <v>1.1499999999999999</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F46" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G46" s="32"/>
+      <c r="G46" s="46"/>
     </row>
     <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="36"/>
+      <c r="A47" s="57"/>
       <c r="B47" s="19" t="s">
         <v>58</v>
       </c>
@@ -2005,28 +1998,28 @@
       <c r="E47" s="28">
         <v>1</v>
       </c>
-      <c r="F47" s="42" t="s">
+      <c r="F47" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G47" s="43"/>
+      <c r="G47" s="68"/>
     </row>
     <row r="48" spans="1:7" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
+      <c r="A48" s="57"/>
       <c r="B48" s="20"/>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
       <c r="E48" s="28"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="30"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="70"/>
     </row>
     <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
+      <c r="A49" s="58"/>
       <c r="B49" s="20"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
       <c r="E49" s="28"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="30"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="70"/>
     </row>
     <row r="50" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
@@ -2034,129 +2027,133 @@
       <c r="C50" s="16"/>
       <c r="D50" s="17"/>
       <c r="E50" s="18"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="30"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="70"/>
     </row>
     <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38" t="s">
+      <c r="B51" s="64"/>
+      <c r="C51" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="41">
+      <c r="D51" s="66">
         <v>3</v>
       </c>
-      <c r="E51" s="54"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="51"/>
+      <c r="E51" s="76">
+        <v>3</v>
+      </c>
+      <c r="F51" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="G51" s="73"/>
     </row>
     <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="36"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="53"/>
+      <c r="A52" s="57"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="77"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="75"/>
     </row>
     <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="36"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="53"/>
+      <c r="A53" s="57"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="75"/>
     </row>
     <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="36"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="53"/>
+      <c r="A54" s="57"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="77"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="75"/>
     </row>
     <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="69"/>
-      <c r="B55" s="70"/>
-      <c r="C55" s="73"/>
-      <c r="D55" s="73"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="70"/>
-      <c r="G55" s="40"/>
+      <c r="A55" s="62"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="63"/>
     </row>
     <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="44" t="s">
+      <c r="A56" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="72"/>
-      <c r="C56" s="79" t="s">
+      <c r="B56" s="38"/>
+      <c r="C56" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="D56" s="79">
+      <c r="D56" s="35">
         <v>45</v>
       </c>
-      <c r="E56" s="74" t="s">
+      <c r="E56" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F56" s="47" t="s">
+      <c r="F56" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="G56" s="48"/>
+      <c r="G56" s="44"/>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
-      <c r="B57" s="73"/>
-      <c r="C57" s="76" t="s">
+      <c r="A57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="D57" s="76">
-        <v>2</v>
-      </c>
-      <c r="E57" s="75">
+      <c r="D57" s="32">
+        <v>0</v>
+      </c>
+      <c r="E57" s="31">
         <f>(D57/D56)</f>
-        <v>4.4444444444444446E-2</v>
-      </c>
-      <c r="F57" s="61">
+        <v>0</v>
+      </c>
+      <c r="F57" s="50">
         <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
-        <v>57.8</v>
-      </c>
-      <c r="G57" s="62"/>
+        <v>67.8</v>
+      </c>
+      <c r="G57" s="51"/>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="45"/>
-      <c r="B58" s="73"/>
-      <c r="C58" s="77" t="s">
+      <c r="A58" s="39"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="D58" s="77">
-        <v>3</v>
-      </c>
-      <c r="E58" s="75">
+      <c r="D58" s="33">
+        <v>0</v>
+      </c>
+      <c r="E58" s="31">
         <f>D58/D56</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="F58" s="63"/>
-      <c r="G58" s="64"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="52"/>
+      <c r="G58" s="53"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="46"/>
-      <c r="B59" s="70"/>
-      <c r="C59" s="78" t="s">
+      <c r="A59" s="41"/>
+      <c r="B59" s="42"/>
+      <c r="C59" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D59" s="78">
-        <v>40</v>
-      </c>
-      <c r="E59" s="75">
+      <c r="D59" s="34">
+        <v>45</v>
+      </c>
+      <c r="E59" s="31">
         <f>D59/D56</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F59" s="65"/>
-      <c r="G59" s="66"/>
+        <v>1</v>
+      </c>
+      <c r="F59" s="54"/>
+      <c r="G59" s="55"/>
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F61" s="22"/>
@@ -5968,6 +5965,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
     <mergeCell ref="A56:B59"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="F17:G17"/>
@@ -5984,56 +6028,9 @@
     <mergeCell ref="A2:A21"/>
     <mergeCell ref="A23:A42"/>
     <mergeCell ref="A44:A49"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F44:F49 F1:F21 F23:F42 F61:G1012" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F44:F49 F1:F21 F61:G1012 F23:F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Doing,Done,To do"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6050,7 +6047,7 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -6089,7 +6086,7 @@
       </c>
       <c r="D2" s="26">
         <f>WP!E9 + WP!E11 + WP!E18 + WP!E20 + WP!E30 + WP!E32 + WP!E39 + WP!E41 + WP!E47 + WP!E51</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6105,7 +6102,7 @@
       </c>
       <c r="D3" s="26">
         <f>WP!E8 + WP!E10 + WP!E14 + WP!E16 + WP!E29 + WP!E31 + WP!E35 + WP!E37</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6137,7 +6134,7 @@
       </c>
       <c r="D5" s="26">
         <f>WP!E4 + WP!E6 + WP!E19 + WP!E21 + WP!E25 + WP!E27 + WP!E40 + WP!E42</f>
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6157,7 +6154,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="36" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="27">
@@ -6170,7 +6167,7 @@
       </c>
       <c r="D7" s="27">
         <f>D2+D3+D4+D5+D6</f>
-        <v>57.8</v>
+        <v>67.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>